<commit_message>
updated operator instructions.py and chapter_functions.py to fix bug that wouldn't print all operator instructions work packages properly.
</commit_message>
<xml_diff>
--- a/trackers/-12&P TM Tracker.xlsx
+++ b/trackers/-12&P TM Tracker.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\TM-Generator\trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA80613-0C56-42D1-ACA3-69D85B3653F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B9B60E-51DA-4F81-A30D-A823BF197448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52095" yWindow="12375" windowWidth="15390" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="-13&amp;P" sheetId="2" r:id="rId1"/>
+    <sheet name="-12&amp;P" sheetId="2" r:id="rId1"/>
     <sheet name="Chapters" sheetId="3" r:id="rId2"/>
     <sheet name="Procedures" sheetId="4" r:id="rId3"/>
     <sheet name="Conditions" sheetId="5" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="188">
   <si>
     <t>Title Page</t>
   </si>
@@ -256,9 +256,6 @@
     <t>WP NO:</t>
   </si>
   <si>
-    <t>PROCEDURE</t>
-  </si>
-  <si>
     <t>TITLE</t>
   </si>
   <si>
@@ -553,9 +550,6 @@
     <t>Operating Procedures</t>
   </si>
   <si>
-    <t>CONDITION</t>
-  </si>
-  <si>
     <t>secref</t>
   </si>
   <si>
@@ -581,6 +575,18 @@
   </si>
   <si>
     <t>Conditions</t>
+  </si>
+  <si>
+    <t>CONDITIONS</t>
+  </si>
+  <si>
+    <t>PROCEDURES</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Should this be site or prepforuse?</t>
   </si>
 </sst>
 </file>
@@ -764,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -822,6 +828,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1179,36 +1191,41 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="6" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -1217,7 +1234,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
@@ -1226,7 +1243,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
@@ -1235,7 +1252,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
@@ -1244,7 +1261,7 @@
       <c r="D5" s="14"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
@@ -1253,7 +1270,7 @@
       <c r="D6" s="14"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
@@ -1262,7 +1279,7 @@
       <c r="D7" s="15"/>
       <c r="E7" s="20"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
         <v>6</v>
@@ -1273,7 +1290,7 @@
       <c r="D8" s="14"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
@@ -1284,7 +1301,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
         <v>10</v>
@@ -1295,16 +1312,16 @@
       <c r="D10" s="14"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
@@ -1315,7 +1332,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
@@ -1325,10 +1342,13 @@
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
@@ -1338,10 +1358,10 @@
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>51</v>
@@ -1351,26 +1371,26 @@
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>16</v>
@@ -1382,7 +1402,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="20"/>
@@ -1446,7 +1466,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="20"/>
@@ -1499,7 +1519,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="20"/>
@@ -1513,7 +1533,7 @@
         <v>65</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="21"/>
     </row>
@@ -1526,7 +1546,7 @@
         <v>24</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E31" s="21"/>
     </row>
@@ -1539,7 +1559,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E32" s="21"/>
     </row>
@@ -1552,7 +1572,7 @@
         <v>66</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" s="21"/>
     </row>
@@ -1565,7 +1585,7 @@
         <v>67</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E34" s="21"/>
     </row>
@@ -1578,7 +1598,7 @@
         <v>67</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E35" s="21"/>
     </row>
@@ -1591,7 +1611,7 @@
         <v>68</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" s="21"/>
     </row>
@@ -1599,7 +1619,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="10"/>
       <c r="C37" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="20"/>
@@ -1607,7 +1627,7 @@
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>54</v>
@@ -1618,7 +1638,7 @@
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>55</v>
@@ -1629,7 +1649,7 @@
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>56</v>
@@ -1640,7 +1660,7 @@
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>58</v>
@@ -1651,7 +1671,7 @@
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>60</v>
@@ -1663,7 +1683,7 @@
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="20"/>
@@ -1671,7 +1691,7 @@
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>21</v>
@@ -1682,7 +1702,7 @@
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>61</v>
@@ -1693,7 +1713,7 @@
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>62</v>
@@ -1704,7 +1724,7 @@
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>63</v>
@@ -1715,7 +1735,7 @@
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>64</v>
@@ -1727,7 +1747,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="20"/>
@@ -1735,10 +1755,10 @@
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="21"/>
@@ -1746,85 +1766,85 @@
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E51" s="21"/>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E52" s="21"/>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E53" s="21"/>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>67</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E55" s="21"/>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
       <c r="C57" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="20"/>
@@ -1844,7 +1864,7 @@
         <v>35</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D59" s="14"/>
       <c r="E59" s="21"/>
@@ -1854,7 +1874,7 @@
         <v>69</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="21"/>
@@ -1862,77 +1882,77 @@
     <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
       <c r="C61" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="20"/>
     </row>
     <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="21"/>
     </row>
     <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="21"/>
     </row>
     <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="21"/>
     </row>
     <row r="65" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D66" s="14"/>
       <c r="E66" s="21"/>
     </row>
     <row r="67" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="21"/>
     </row>
     <row r="68" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B68" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="21"/>
@@ -1940,7 +1960,7 @@
     <row r="69" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
       <c r="C69" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="20"/>
@@ -1960,7 +1980,7 @@
         <v>38</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="21"/>
@@ -1970,7 +1990,7 @@
         <v>40</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D72" s="14"/>
       <c r="E72" s="21"/>
@@ -2037,7 +2057,7 @@
     </row>
     <row r="79" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B79" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>74</v>
@@ -2047,7 +2067,7 @@
     </row>
     <row r="80" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B80" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>45</v>
@@ -2108,7 +2128,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -2118,57 +2138,57 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
@@ -2199,228 +2219,228 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2446,52 +2466,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>